<commit_message>
adding xlsx graph for model 2
</commit_message>
<xml_diff>
--- a/figures/pop_sims/pop_sim_skaakai/data_output_simu_model1.xlsx
+++ b/figures/pop_sims/pop_sim_skaakai/data_output_simu_model1.xlsx
@@ -14,39 +14,6 @@
   <sheets>
     <sheet name="data_output_simu_model1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">data_output_simu_model1!$DD$17:$EF$17</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">data_output_simu_model1!$DD$18:$EF$18</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">data_output_simu_model1!$DD$2:$DS$2</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">data_output_simu_model1!$DC$1:$DS$1</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">data_output_simu_model1!$DC$2</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">data_output_simu_model1!$DC$2:$DS$2</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">data_output_simu_model1!$DC$3:$DS$3</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">data_output_simu_model1!$DC$4:$DS$4</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">data_output_simu_model1!$DC$5:$DS$5</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">data_output_simu_model1!$DD$1:$DS$1</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">data_output_simu_model1!$DD$2:$DS$2</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">data_output_simu_model1!$DD$3:$DS$3</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">data_output_simu_model1!$DD$19:$EF$19</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">data_output_simu_model1!$DD$4:$DS$4</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">data_output_simu_model1!$DD$5:$DS$5</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">data_output_simu_model1!$DC$17:$DT$17</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">data_output_simu_model1!$DC$18:$DT$18</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">data_output_simu_model1!$DC$19:$DT$19</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">data_output_simu_model1!$DC$20:$DT$20</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">data_output_simu_model1!$DC$21:$DT$21</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">data_output_simu_model1!$DC$22:$DT$22</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">data_output_simu_model1!$DC$23:$DT$23</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">data_output_simu_model1!$DC$24:$DT$24</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">data_output_simu_model1!$DD$20:$EF$20</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">data_output_simu_model1!$DC$25:$DT$25</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">data_output_simu_model1!$DD$21:$EF$21</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">data_output_simu_model1!$DD$22:$EF$22</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">data_output_simu_model1!$DD$23:$EF$23</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">data_output_simu_model1!$DD$24:$EF$24</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">data_output_simu_model1!$DD$25:$EF$25</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">data_output_simu_model1!$DD$1:$DS$1</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -1150,11 +1117,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>data_output_simu_model1!$F$17</c:f>
+              <c:f>data_output_simu_model1!$F$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0,01</c:v>
+                  <c:v>0,1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1343,159 +1310,159 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>data_output_simu_model1!$G$17:$BD$17</c:f>
+              <c:f>data_output_simu_model1!$G$27:$BD$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>56</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>63</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>72</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>80</c:v>
+                  <c:v>182</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>85</c:v>
+                  <c:v>198</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>96</c:v>
+                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>98</c:v>
+                  <c:v>237</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>101</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>104</c:v>
+                  <c:v>292</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>105</c:v>
+                  <c:v>329</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>107</c:v>
+                  <c:v>362</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>110</c:v>
+                  <c:v>399</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>119</c:v>
+                  <c:v>442</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>124</c:v>
+                  <c:v>458</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>121</c:v>
+                  <c:v>484</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>128</c:v>
+                  <c:v>517</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>125</c:v>
+                  <c:v>561</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>124</c:v>
+                  <c:v>599</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>121</c:v>
+                  <c:v>641</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>125</c:v>
+                  <c:v>687</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>122</c:v>
+                  <c:v>732</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>123</c:v>
+                  <c:v>782</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>129</c:v>
+                  <c:v>834</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>134</c:v>
+                  <c:v>896</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>139</c:v>
+                  <c:v>954</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>137</c:v>
+                  <c:v>1008</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>141</c:v>
+                  <c:v>1079</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>131</c:v>
+                  <c:v>1138</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>130</c:v>
+                  <c:v>1182</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>135</c:v>
+                  <c:v>1247</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>134</c:v>
+                  <c:v>1353</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>136</c:v>
+                  <c:v>1441</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>141</c:v>
+                  <c:v>1530</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>139</c:v>
+                  <c:v>1629</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>137</c:v>
+                  <c:v>1704</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>137</c:v>
+                  <c:v>1793</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>136</c:v>
+                  <c:v>1875</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>138</c:v>
+                  <c:v>1989</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>141</c:v>
+                  <c:v>2097</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>138</c:v>
+                  <c:v>2182</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>135</c:v>
+                  <c:v>2298</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>133</c:v>
+                  <c:v>2431</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>136</c:v>
+                  <c:v>2532</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1512,11 +1479,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>data_output_simu_model1!$F$18</c:f>
+              <c:f>data_output_simu_model1!$F$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0,1</c:v>
+                  <c:v>0,2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1705,159 +1672,159 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>data_output_simu_model1!$G$18:$BD$18</c:f>
+              <c:f>data_output_simu_model1!$G$28:$BD$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>49</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>66</c:v>
+                  <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>91</c:v>
+                  <c:v>172</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>108</c:v>
+                  <c:v>221</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>121</c:v>
+                  <c:v>275</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>133</c:v>
+                  <c:v>348</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>152</c:v>
+                  <c:v>416</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>174</c:v>
+                  <c:v>498</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>193</c:v>
+                  <c:v>591</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>206</c:v>
+                  <c:v>717</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>226</c:v>
+                  <c:v>854</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>241</c:v>
+                  <c:v>1007</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>256</c:v>
+                  <c:v>1209</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>286</c:v>
+                  <c:v>1456</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>305</c:v>
+                  <c:v>1747</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>338</c:v>
+                  <c:v>2073</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>364</c:v>
+                  <c:v>2456</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>407</c:v>
+                  <c:v>2863</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>431</c:v>
+                  <c:v>3360</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>486</c:v>
+                  <c:v>3865</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>533</c:v>
+                  <c:v>4488</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>584</c:v>
+                  <c:v>5108</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>624</c:v>
+                  <c:v>5833</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>677</c:v>
+                  <c:v>6570</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>717</c:v>
+                  <c:v>7355</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>764</c:v>
+                  <c:v>8212</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>838</c:v>
+                  <c:v>9071</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>910</c:v>
+                  <c:v>9878</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>966</c:v>
+                  <c:v>10668</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1041</c:v>
+                  <c:v>11400</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1118</c:v>
+                  <c:v>12030</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1226</c:v>
+                  <c:v>12847</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1318</c:v>
+                  <c:v>13519</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1398</c:v>
+                  <c:v>14186</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1529</c:v>
+                  <c:v>14881</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1627</c:v>
+                  <c:v>15415</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1745</c:v>
+                  <c:v>15770</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1865</c:v>
+                  <c:v>15996</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2007</c:v>
+                  <c:v>16380</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2155</c:v>
+                  <c:v>16709</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2306</c:v>
+                  <c:v>16998</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2468</c:v>
+                  <c:v>17153</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2624</c:v>
+                  <c:v>17377</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2782</c:v>
+                  <c:v>17470</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1874,11 +1841,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>data_output_simu_model1!$F$19</c:f>
+              <c:f>data_output_simu_model1!$F$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0,2</c:v>
+                  <c:v>0,3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2067,159 +2034,159 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>data_output_simu_model1!$G$19:$BD$19</c:f>
+              <c:f>data_output_simu_model1!$G$29:$BD$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>47</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>72</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>94</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>123</c:v>
+                  <c:v>172</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>151</c:v>
+                  <c:v>222</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>185</c:v>
+                  <c:v>319</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>234</c:v>
+                  <c:v>417</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>280</c:v>
+                  <c:v>569</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>340</c:v>
+                  <c:v>737</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>422</c:v>
+                  <c:v>984</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>509</c:v>
+                  <c:v>1313</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>618</c:v>
+                  <c:v>1781</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>765</c:v>
+                  <c:v>2303</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>906</c:v>
+                  <c:v>2993</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1098</c:v>
+                  <c:v>3832</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1295</c:v>
+                  <c:v>4874</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1577</c:v>
+                  <c:v>6181</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1891</c:v>
+                  <c:v>7729</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2276</c:v>
+                  <c:v>9418</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2754</c:v>
+                  <c:v>11318</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3297</c:v>
+                  <c:v>13260</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3917</c:v>
+                  <c:v>15268</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4707</c:v>
+                  <c:v>17293</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5658</c:v>
+                  <c:v>19300</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>6805</c:v>
+                  <c:v>21025</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>8057</c:v>
+                  <c:v>22672</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>9600</c:v>
+                  <c:v>23997</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>11348</c:v>
+                  <c:v>25165</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>13495</c:v>
+                  <c:v>26019</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>15936</c:v>
+                  <c:v>26618</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>18799</c:v>
+                  <c:v>27183</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>22116</c:v>
+                  <c:v>27606</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>25949</c:v>
+                  <c:v>27606</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>30364</c:v>
+                  <c:v>27754</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>35516</c:v>
+                  <c:v>28159</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>40968</c:v>
+                  <c:v>28388</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>47167</c:v>
+                  <c:v>28639</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>53764</c:v>
+                  <c:v>28705</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>60927</c:v>
+                  <c:v>28979</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>68841</c:v>
+                  <c:v>29151</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>76700</c:v>
+                  <c:v>29047</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>84915</c:v>
+                  <c:v>28934</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>93287</c:v>
+                  <c:v>28879</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>101679</c:v>
+                  <c:v>28959</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>109604</c:v>
+                  <c:v>28670</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>117274</c:v>
+                  <c:v>28740</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>124640</c:v>
+                  <c:v>28767</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>131654</c:v>
+                  <c:v>28860</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2236,11 +2203,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>data_output_simu_model1!$F$20</c:f>
+              <c:f>data_output_simu_model1!$F$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0,3</c:v>
+                  <c:v>0,4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2429,7 +2396,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>data_output_simu_model1!$G$20:$BD$20</c:f>
+              <c:f>data_output_simu_model1!$G$30:$BD$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -2437,151 +2404,151 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>101</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>157</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>213</c:v>
+                  <c:v>314</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>295</c:v>
+                  <c:v>448</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>403</c:v>
+                  <c:v>685</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>548</c:v>
+                  <c:v>1012</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>772</c:v>
+                  <c:v>1470</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1050</c:v>
+                  <c:v>2217</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1407</c:v>
+                  <c:v>3199</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1900</c:v>
+                  <c:v>4567</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2536</c:v>
+                  <c:v>6531</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3374</c:v>
+                  <c:v>9057</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4532</c:v>
+                  <c:v>12085</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6097</c:v>
+                  <c:v>15642</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8125</c:v>
+                  <c:v>19558</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10817</c:v>
+                  <c:v>23379</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>14185</c:v>
+                  <c:v>26929</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>18641</c:v>
+                  <c:v>29940</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>24493</c:v>
+                  <c:v>32635</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>31747</c:v>
+                  <c:v>34508</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>40976</c:v>
+                  <c:v>35942</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>52205</c:v>
+                  <c:v>37044</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>65788</c:v>
+                  <c:v>37611</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>81658</c:v>
+                  <c:v>38131</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>99506</c:v>
+                  <c:v>38466</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>119342</c:v>
+                  <c:v>38749</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>140102</c:v>
+                  <c:v>39102</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>161190</c:v>
+                  <c:v>39198</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>181725</c:v>
+                  <c:v>39220</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>200762</c:v>
+                  <c:v>39172</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>217524</c:v>
+                  <c:v>39355</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>231790</c:v>
+                  <c:v>39125</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>244289</c:v>
+                  <c:v>39379</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>254642</c:v>
+                  <c:v>39226</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>262267</c:v>
+                  <c:v>39459</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>269013</c:v>
+                  <c:v>39291</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>274059</c:v>
+                  <c:v>39504</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>277632</c:v>
+                  <c:v>39591</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>280738</c:v>
+                  <c:v>39655</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>283607</c:v>
+                  <c:v>39430</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>284996</c:v>
+                  <c:v>39397</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>286623</c:v>
+                  <c:v>39520</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>287093</c:v>
+                  <c:v>39532</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>287967</c:v>
+                  <c:v>39502</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>288575</c:v>
+                  <c:v>39312</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>288992</c:v>
+                  <c:v>39340</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2590,1834 +2557,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-643E-4EFA-8964-DE8990D9D81A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>data_output_simu_model1!$F$21</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0,4</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:strRef>
-              <c:f>data_output_simu_model1!$G$1:$BD$1</c:f>
-              <c:strCache>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>n_alive_0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>n_alive_1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>n_alive_2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>n_alive_3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>n_alive_4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>n_alive_5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>n_alive_6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>n_alive_7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>n_alive_8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>n_alive_9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>n_alive_10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>n_alive_11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>n_alive_12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>n_alive_13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>n_alive_14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>n_alive_15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>n_alive_16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>n_alive_17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>n_alive_18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>n_alive_19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>n_alive_20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>n_alive_21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>n_alive_22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>n_alive_23</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>n_alive_24</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>n_alive_25</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>n_alive_26</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>n_alive_27</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>n_alive_28</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>n_alive_29</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>n_alive_30</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>n_alive_31</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>n_alive_32</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>n_alive_33</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>n_alive_34</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>n_alive_35</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>n_alive_36</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>n_alive_37</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>n_alive_38</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>n_alive_39</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>n_alive_40</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>n_alive_41</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>n_alive_42</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>n_alive_43</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>n_alive_44</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>n_alive_45</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>n_alive_46</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>n_alive_47</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>n_alive_48</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>n_alive_49</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>data_output_simu_model1!$G$21:$BD$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>83</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>135</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>340</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>503</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>736</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1038</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1469</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2171</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3204</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4772</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7046</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>10196</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>15001</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>21682</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>31417</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>44709</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>62708</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>86366</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>116141</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>150808</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>188408</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>226608</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>263394</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>294808</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>321471</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>342297</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>356961</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>369035</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>376869</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>381556</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>385484</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>388410</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>389081</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>390625</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>391944</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>392335</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>392351</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>392717</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>393000</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>393431</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>394334</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>395007</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>394493</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>393593</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>393738</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>394107</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000010-643E-4EFA-8964-DE8990D9D81A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>data_output_simu_model1!$F$22</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0,5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:strRef>
-              <c:f>data_output_simu_model1!$G$1:$BD$1</c:f>
-              <c:strCache>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>n_alive_0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>n_alive_1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>n_alive_2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>n_alive_3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>n_alive_4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>n_alive_5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>n_alive_6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>n_alive_7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>n_alive_8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>n_alive_9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>n_alive_10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>n_alive_11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>n_alive_12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>n_alive_13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>n_alive_14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>n_alive_15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>n_alive_16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>n_alive_17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>n_alive_18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>n_alive_19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>n_alive_20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>n_alive_21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>n_alive_22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>n_alive_23</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>n_alive_24</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>n_alive_25</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>n_alive_26</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>n_alive_27</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>n_alive_28</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>n_alive_29</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>n_alive_30</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>n_alive_31</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>n_alive_32</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>n_alive_33</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>n_alive_34</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>n_alive_35</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>n_alive_36</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>n_alive_37</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>n_alive_38</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>n_alive_39</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>n_alive_40</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>n_alive_41</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>n_alive_42</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>n_alive_43</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>n_alive_44</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>n_alive_45</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>n_alive_46</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>n_alive_47</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>n_alive_48</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>n_alive_49</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>data_output_simu_model1!$G$22:$BD$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>127</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>209</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>357</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>574</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>967</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1590</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2620</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4277</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7030</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>11381</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>18530</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>29943</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>47363</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>73453</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>110012</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>158425</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>215621</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>277004</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>334786</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>383725</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>420906</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>447971</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>466396</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>477796</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>484521</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>488883</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>490695</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>493468</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>494114</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>494834</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>496367</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>495604</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>494998</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>495198</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>495389</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>495239</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>496623</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>495966</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>496402</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>495982</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>495826</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>496490</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>496399</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>496036</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>495681</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>496277</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>496718</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000011-643E-4EFA-8964-DE8990D9D81A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>data_output_simu_model1!$F$23</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0,6</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:strRef>
-              <c:f>data_output_simu_model1!$G$1:$BD$1</c:f>
-              <c:strCache>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>n_alive_0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>n_alive_1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>n_alive_2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>n_alive_3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>n_alive_4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>n_alive_5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>n_alive_6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>n_alive_7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>n_alive_8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>n_alive_9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>n_alive_10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>n_alive_11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>n_alive_12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>n_alive_13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>n_alive_14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>n_alive_15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>n_alive_16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>n_alive_17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>n_alive_18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>n_alive_19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>n_alive_20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>n_alive_21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>n_alive_22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>n_alive_23</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>n_alive_24</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>n_alive_25</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>n_alive_26</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>n_alive_27</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>n_alive_28</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>n_alive_29</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>n_alive_30</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>n_alive_31</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>n_alive_32</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>n_alive_33</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>n_alive_34</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>n_alive_35</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>n_alive_36</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>n_alive_37</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>n_alive_38</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>n_alive_39</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>n_alive_40</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>n_alive_41</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>n_alive_42</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>n_alive_43</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>n_alive_44</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>n_alive_45</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>n_alive_46</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>n_alive_47</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>n_alive_48</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>n_alive_49</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>data_output_simu_model1!$G$23:$BD$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>107</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>194</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>352</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>661</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1215</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2135</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3776</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6848</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12377</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>22047</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>38889</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>67462</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>112562</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>177329</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>258473</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>347311</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>427567</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>490331</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>534333</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>561112</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>576895</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>586309</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>591177</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>593761</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>594465</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>595680</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>596413</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>596005</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>596475</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>597659</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>597113</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>596231</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>597098</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>598550</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>597626</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>597526</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>596590</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>597338</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>598085</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>597111</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>596607</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>596523</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>596435</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>596955</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>596771</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>597207</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>596685</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000012-643E-4EFA-8964-DE8990D9D81A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>data_output_simu_model1!$F$24</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0,7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:strRef>
-              <c:f>data_output_simu_model1!$G$1:$BD$1</c:f>
-              <c:strCache>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>n_alive_0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>n_alive_1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>n_alive_2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>n_alive_3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>n_alive_4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>n_alive_5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>n_alive_6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>n_alive_7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>n_alive_8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>n_alive_9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>n_alive_10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>n_alive_11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>n_alive_12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>n_alive_13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>n_alive_14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>n_alive_15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>n_alive_16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>n_alive_17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>n_alive_18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>n_alive_19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>n_alive_20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>n_alive_21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>n_alive_22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>n_alive_23</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>n_alive_24</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>n_alive_25</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>n_alive_26</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>n_alive_27</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>n_alive_28</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>n_alive_29</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>n_alive_30</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>n_alive_31</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>n_alive_32</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>n_alive_33</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>n_alive_34</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>n_alive_35</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>n_alive_36</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>n_alive_37</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>n_alive_38</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>n_alive_39</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>n_alive_40</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>n_alive_41</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>n_alive_42</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>n_alive_43</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>n_alive_44</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>n_alive_45</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>n_alive_46</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>n_alive_47</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>n_alive_48</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>n_alive_49</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>data_output_simu_model1!$G$24:$BD$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>116</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>232</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>496</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>965</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1910</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3887</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7764</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>15459</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>30266</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>58170</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>107889</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>188439</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>297816</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>417359</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>524110</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>598212</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>644889</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>669958</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>683516</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>690162</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>693612</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>694345</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>695632</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>697105</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>698312</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>699366</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>697844</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>697457</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>696721</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>697523</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>697813</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>698418</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>697766</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>697781</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>698833</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>699006</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>698299</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>697256</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>698819</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>697798</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>698167</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>696847</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>698183</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>698409</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>698191</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>698030</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>698291</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>696718</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000013-643E-4EFA-8964-DE8990D9D81A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="8"/>
-          <c:order val="8"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>data_output_simu_model1!$F$25</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0,8</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:strRef>
-              <c:f>data_output_simu_model1!$G$1:$BD$1</c:f>
-              <c:strCache>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>n_alive_0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>n_alive_1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>n_alive_2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>n_alive_3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>n_alive_4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>n_alive_5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>n_alive_6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>n_alive_7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>n_alive_8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>n_alive_9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>n_alive_10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>n_alive_11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>n_alive_12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>n_alive_13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>n_alive_14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>n_alive_15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>n_alive_16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>n_alive_17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>n_alive_18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>n_alive_19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>n_alive_20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>n_alive_21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>n_alive_22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>n_alive_23</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>n_alive_24</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>n_alive_25</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>n_alive_26</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>n_alive_27</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>n_alive_28</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>n_alive_29</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>n_alive_30</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>n_alive_31</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>n_alive_32</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>n_alive_33</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>n_alive_34</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>n_alive_35</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>n_alive_36</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>n_alive_37</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>n_alive_38</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>n_alive_39</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>n_alive_40</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>n_alive_41</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>n_alive_42</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>n_alive_43</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>n_alive_44</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>n_alive_45</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>n_alive_46</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>n_alive_47</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>n_alive_48</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>n_alive_49</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>data_output_simu_model1!$G$25:$BD$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>116</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>272</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>622</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1417</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3124</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6922</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>15521</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>33778</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>71407</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>142382</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>260106</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>412547</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>561368</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>670735</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>735385</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>769159</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>784365</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>792650</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>797196</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>796867</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>797437</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>797473</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>797354</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>799370</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>799886</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>799958</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>798844</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>797673</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>797761</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>798365</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>798343</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>799172</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>798984</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>798474</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>796981</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>797338</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>798382</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>798487</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>798018</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>796646</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>797769</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>798684</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>797887</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>798192</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>798509</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>798090</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>798910</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>799463</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000014-643E-4EFA-8964-DE8990D9D81A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4712,7 +2851,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>data_output_simu_model1!$BE$17:$DB$17</c:f>
+              <c:f>data_output_simu_model1!$BE$27:$DB$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -4720,151 +2859,151 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.5238095238095205E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.2</c:v>
+                  <c:v>8.5714285714285701E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.13793103448275901</c:v>
+                  <c:v>7.4074074074074098E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14285714285714299</c:v>
+                  <c:v>7.8125E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.16666666666666699</c:v>
+                  <c:v>4.5454545454545497E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.15094339622641501</c:v>
+                  <c:v>6.5420560747663503E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.17857142857142899</c:v>
+                  <c:v>7.8125E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.206349206349206</c:v>
+                  <c:v>8.5714285714285701E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.25</c:v>
+                  <c:v>0.113207547169811</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.23749999999999999</c:v>
+                  <c:v>0.12637362637362601</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.27058823529411802</c:v>
+                  <c:v>0.11616161616161599</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.25</c:v>
+                  <c:v>0.100456621004566</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.23469387755102</c:v>
+                  <c:v>0.10126582278481</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.26732673267326701</c:v>
+                  <c:v>0.111538461538462</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.27884615384615402</c:v>
+                  <c:v>0.10958904109589</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.22857142857142901</c:v>
+                  <c:v>0.100303951367781</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.26168224299065401</c:v>
+                  <c:v>0.113259668508287</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.263636363636364</c:v>
+                  <c:v>0.12280701754386</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.24369747899159699</c:v>
+                  <c:v>0.131221719457014</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.29032258064516098</c:v>
+                  <c:v>0.14192139737991299</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.256198347107438</c:v>
+                  <c:v>0.14669421487603301</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.2421875</c:v>
+                  <c:v>0.145067698259188</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.27200000000000002</c:v>
+                  <c:v>0.14795008912655999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.29032258064516098</c:v>
+                  <c:v>0.141903171953255</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.28925619834710697</c:v>
+                  <c:v>0.135725429017161</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.30399999999999999</c:v>
+                  <c:v>0.14119359534206699</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.30327868852459</c:v>
+                  <c:v>0.135245901639344</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.284552845528455</c:v>
+                  <c:v>0.132992327365729</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.25581395348837199</c:v>
+                  <c:v>0.12829736211031201</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.28358208955223901</c:v>
+                  <c:v>0.13504464285714299</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.25179856115107901</c:v>
+                  <c:v>0.12788259958071299</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.29927007299270098</c:v>
+                  <c:v>0.121031746031746</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.32624113475177302</c:v>
+                  <c:v>0.13438368860055599</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.33587786259542002</c:v>
+                  <c:v>0.13005272407732901</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.33076923076923098</c:v>
+                  <c:v>0.14128595600676799</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.30370370370370398</c:v>
+                  <c:v>0.13873295910184399</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.31343283582089598</c:v>
+                  <c:v>0.133776792313378</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.308823529411765</c:v>
+                  <c:v>0.13254684247050699</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.30496453900709197</c:v>
+                  <c:v>0.13725490196078399</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.28776978417266202</c:v>
+                  <c:v>0.137507673419276</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.29927007299270098</c:v>
+                  <c:v>0.129107981220657</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.27737226277372301</c:v>
+                  <c:v>0.12716118237590601</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.36029411764705899</c:v>
+                  <c:v>0.12640000000000001</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.34057971014492799</c:v>
+                  <c:v>0.12569130216189001</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.37588652482269502</c:v>
+                  <c:v>0.13066285169289499</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.36956521739130399</c:v>
+                  <c:v>0.13519706691109101</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.38518518518518502</c:v>
+                  <c:v>0.134029590948651</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.37593984962406002</c:v>
+                  <c:v>0.13368983957219299</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.38235294117647101</c:v>
+                  <c:v>0.127172195892575</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4905,7 +3044,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>data_output_simu_model1!$BE$18:$DB$18</c:f>
+              <c:f>data_output_simu_model1!$BE$28:$DB$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -4913,151 +3052,151 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5.2631578947368397E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.12121212121212099</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11363636363636399</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.138461538461538</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13750000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.12631578947368399</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.1603053435114504E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.9767441860465101E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>7.69230769230769E-2</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.0909090909090898E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.3170731707317097E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.102040816326531</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.105263157894737</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.0909090909090898E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.13186813186813201</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.13888888888888901</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.14049586776859499</c:v>
+                  <c:v>6.5454545454545501E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.150375939849624</c:v>
+                  <c:v>6.6091954022988494E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.15131578947368399</c:v>
+                  <c:v>7.93269230769231E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.14367816091954</c:v>
+                  <c:v>6.82730923694779E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.14507772020725401</c:v>
+                  <c:v>6.0913705583756299E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.12621359223301001</c:v>
+                  <c:v>6.9735006973500699E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.123893805309735</c:v>
+                  <c:v>5.7377049180327898E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.145228215767635</c:v>
+                  <c:v>5.8589870903674297E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.14453125</c:v>
+                  <c:v>5.0454921422663397E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.15034965034965</c:v>
+                  <c:v>4.1895604395604399E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.150819672131148</c:v>
+                  <c:v>5.3806525472238097E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.14201183431952699</c:v>
+                  <c:v>5.45103714423541E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.12637362637362601</c:v>
+                  <c:v>5.74104234527687E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.100737100737101</c:v>
+                  <c:v>5.4488298987076501E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.111368909512761</c:v>
+                  <c:v>5.2678571428571401E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.109053497942387</c:v>
+                  <c:v>5.22639068564036E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.120075046904315</c:v>
+                  <c:v>5.3921568627450997E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.118150684931507</c:v>
+                  <c:v>5.16836335160532E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.121794871794872</c:v>
+                  <c:v>4.8859934853420203E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.119645494830133</c:v>
+                  <c:v>5.0684931506849301E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.121338912133891</c:v>
+                  <c:v>4.79945615227736E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.12172774869109899</c:v>
+                  <c:v>4.7856794934242601E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.114558472553699</c:v>
+                  <c:v>4.6742365781060502E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.114285714285714</c:v>
+                  <c:v>4.52520753188905E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.114906832298137</c:v>
+                  <c:v>4.8743907011623497E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.121037463976945</c:v>
+                  <c:v>5.0087719298245598E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.118962432915921</c:v>
+                  <c:v>5.0706566916043201E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.11827079934747101</c:v>
+                  <c:v>4.8727329337588499E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.118361153262519</c:v>
+                  <c:v>4.8746209039130101E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.105865522174535</c:v>
+                  <c:v>4.7864091357676601E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.11772400261608899</c:v>
+                  <c:v>4.7913446676970603E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.123540258143823</c:v>
+                  <c:v>4.9172883554978897E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.122063037249284</c:v>
+                  <c:v>4.7812301838934701E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.12171581769437</c:v>
+                  <c:v>4.8199549887471903E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.120577977080219</c:v>
+                  <c:v>4.5848595848595797E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.122505800464037</c:v>
+                  <c:v>4.4167813753067199E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.12012142237640901</c:v>
+                  <c:v>4.50052947405577E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.121961102106969</c:v>
+                  <c:v>4.4423715968052203E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.123856707317073</c:v>
+                  <c:v>4.4886919491281603E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.13012221423436399</c:v>
+                  <c:v>4.3503148254149998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5098,7 +3237,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>data_output_simu_model1!$BE$19:$DB$19</c:f>
+              <c:f>data_output_simu_model1!$BE$29:$DB$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -5106,151 +3245,151 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.4482758620689703E-2</c:v>
+                  <c:v>2.8571428571428598E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1276595744680899E-2</c:v>
+                  <c:v>7.1428571428571397E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.1666666666666699E-2</c:v>
+                  <c:v>8.4337349397590397E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.2553191489361701E-2</c:v>
+                  <c:v>6.9230769230769207E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.3170731707317097E-2</c:v>
+                  <c:v>4.0697674418604703E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.6225165562913899E-2</c:v>
+                  <c:v>4.0540540540540501E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.5675675675675694E-2</c:v>
+                  <c:v>1.88087774294671E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.9743589743589702E-2</c:v>
+                  <c:v>1.9184652278177498E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.9285714285714302E-2</c:v>
+                  <c:v>2.9876977152899799E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.3529411764705899E-2</c:v>
+                  <c:v>3.2564450474898199E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.1611374407582901E-2</c:v>
+                  <c:v>3.7601626016260201E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.10805500982318E-2</c:v>
+                  <c:v>3.1987814166031997E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.3689320388349502E-2</c:v>
+                  <c:v>2.6951151038742301E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.05228758169935E-2</c:v>
+                  <c:v>2.7789839339991299E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.0772626931567297E-2</c:v>
+                  <c:v>2.7731373204143001E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.7377049180327898E-2</c:v>
+                  <c:v>2.8183716075156601E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.0231660231660197E-2</c:v>
+                  <c:v>2.6466967583094001E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.7070386810399498E-2</c:v>
+                  <c:v>2.3782559456398601E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.0285563194077199E-2</c:v>
+                  <c:v>2.17363177642645E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.7996485061511401E-2</c:v>
+                  <c:v>2.3359524315141201E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.6281771968046498E-2</c:v>
+                  <c:v>2.3590740413500601E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.18653321201092E-2</c:v>
+                  <c:v>2.4208144796380102E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5.1314781720704597E-2</c:v>
+                  <c:v>2.2596279800890798E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5.35372848948375E-2</c:v>
+                  <c:v>2.1800728618516198E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.9487451396253102E-2</c:v>
+                  <c:v>1.98963730569948E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.98163115356356E-2</c:v>
+                  <c:v>1.9928656361474398E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5.0763311406230603E-2</c:v>
+                  <c:v>2.18772053634439E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.9270833333333298E-2</c:v>
+                  <c:v>2.2044422219444099E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.7056750088121303E-2</c:v>
+                  <c:v>2.2133916153387601E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.8165987402741799E-2</c:v>
+                  <c:v>2.1830201006956498E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.7063253012048202E-2</c:v>
+                  <c:v>2.17146291982869E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.7396138092451703E-2</c:v>
+                  <c:v>2.2182982010815599E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.7657804304575897E-2</c:v>
+                  <c:v>2.0937477359994201E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.7631893329222699E-2</c:v>
+                  <c:v>2.0575237267260699E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.6831774469766801E-2</c:v>
+                  <c:v>2.0249333429415602E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.7922063295416199E-2</c:v>
+                  <c:v>2.0100145601761401E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.8379222808045297E-2</c:v>
+                  <c:v>2.1734535719318E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4.7151610235970101E-2</c:v>
+                  <c:v>2.1439296064806702E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.6648314857525498E-2</c:v>
+                  <c:v>2.17383731057307E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4.6481855335073097E-2</c:v>
+                  <c:v>2.0566617205562601E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4.5902877645589098E-2</c:v>
+                  <c:v>2.0994133991972801E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4.5840938722294701E-2</c:v>
+                  <c:v>2.13102902192998E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4.5963610669492998E-2</c:v>
+                  <c:v>2.05640423031727E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4.6308703249113001E-2</c:v>
+                  <c:v>1.9876034488728801E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4.64796073918902E-2</c:v>
+                  <c:v>2.0235505369660602E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4.66588810627349E-2</c:v>
+                  <c:v>2.07534007673526E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4.7009567338028899E-2</c:v>
+                  <c:v>2.1259568545581101E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4.6919127086007699E-2</c:v>
+                  <c:v>2.1795807696318701E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4.6941224725416598E-2</c:v>
+                  <c:v>2.19334719334719E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5291,7 +3430,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>data_output_simu_model1!$BE$20:$DB$20</c:f>
+              <c:f>data_output_simu_model1!$BE$30:$DB$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -5299,151 +3438,151 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.1666666666666699E-2</c:v>
+                  <c:v>3.7037037037037E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.128205128205128</c:v>
+                  <c:v>7.4074074074074098E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.1428571428571397E-2</c:v>
+                  <c:v>4.2553191489361701E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.9009900990099001E-2</c:v>
+                  <c:v>5.7971014492753603E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.7324840764331197E-2</c:v>
+                  <c:v>5.2884615384615398E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.16431924882629E-2</c:v>
+                  <c:v>2.54777070063694E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.0677966101694898E-2</c:v>
+                  <c:v>2.6785714285714302E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.2258064516128997E-2</c:v>
+                  <c:v>2.4817518248175199E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.1021897810218999E-2</c:v>
+                  <c:v>1.58102766798419E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.59067357512953E-2</c:v>
+                  <c:v>1.49659863945578E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.02</c:v>
+                  <c:v>1.44339197113216E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.27434257285004E-2</c:v>
+                  <c:v>1.4692091278524499E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.4210526315789498E-2</c:v>
+                  <c:v>1.2042916575432499E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.5630914826498399E-2</c:v>
+                  <c:v>1.1483693155718899E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.9561351511559001E-2</c:v>
+                  <c:v>1.1151595451032399E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.22859664607237E-2</c:v>
+                  <c:v>1.0757136946628099E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.3946203050680698E-2</c:v>
+                  <c:v>1.0868175425137501E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.2646153846153799E-2</c:v>
+                  <c:v>1.14019838429287E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.2094850697975399E-2</c:v>
+                  <c:v>1.1506052440224099E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.2488544236869901E-2</c:v>
+                  <c:v>1.06205206283189E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.1887237809130398E-2</c:v>
+                  <c:v>1.17234468937876E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.0740619768913601E-2</c:v>
+                  <c:v>1.1827792247586901E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.1230352474249502E-2</c:v>
+                  <c:v>1.2084154398979899E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.21349082389692E-2</c:v>
+                  <c:v>1.1323799454677E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.2124317594100201E-2</c:v>
+                  <c:v>1.11219090810928E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.1660485194868399E-2</c:v>
+                  <c:v>1.1565765334609601E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.14308457224032E-2</c:v>
+                  <c:v>1.05426031313105E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.17474323156393E-2</c:v>
+                  <c:v>1.03467997712265E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.2154815572053399E-2</c:v>
+                  <c:v>1.13293246277323E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.12916303835777E-2</c:v>
+                  <c:v>1.0843435118408301E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.1093119920590601E-2</c:v>
+                  <c:v>1.14291545487015E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.16370890081167E-2</c:v>
+                  <c:v>1.11932687404386E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.1328737510086598E-2</c:v>
+                  <c:v>1.0619830491167199E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.1330979570070401E-2</c:v>
+                  <c:v>1.09770041926058E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.08248845938134E-2</c:v>
+                  <c:v>1.09392971246006E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.1163458035359801E-2</c:v>
+                  <c:v>1.15035932857614E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.1630367339244901E-2</c:v>
+                  <c:v>1.1726915821139E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.1569621797633699E-2</c:v>
+                  <c:v>1.0872044400517001E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2.1292651284510401E-2</c:v>
+                  <c:v>1.0943982082410699E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2.1119539953075799E-2</c:v>
+                  <c:v>1.1543134872418001E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2.13520055325035E-2</c:v>
+                  <c:v>1.16188022530373E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2.1265379107922699E-2</c:v>
+                  <c:v>1.1095700416088801E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2.1156036346070401E-2</c:v>
+                  <c:v>1.1336545777326901E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.0982750635096602E-2</c:v>
+                  <c:v>1.1142980429982E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2.1086933009563099E-2</c:v>
+                  <c:v>1.06528340080972E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2.10767939308865E-2</c:v>
+                  <c:v>1.06496003237883E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2.1030187486760599E-2</c:v>
+                  <c:v>1.1518404131436399E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2.1190331802824199E-2</c:v>
+                  <c:v>1.12688237688238E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2.1194358321337599E-2</c:v>
+                  <c:v>1.16675139806812E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5452,989 +3591,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-961B-4FC7-9B8A-1775915C5FCB}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>data_output_simu_model1!$BE$21:$DB$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.9607843137254902E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.6144578313252997E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.96296296296296E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.2857142857142899E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.7058823529411799E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.78330019880716E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.5815217391304299E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.3121387283237E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.3144996596324002E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.9345923537540301E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.7478152309612999E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.46689019279128E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.43343741129719E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.36327971753629E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.26658222785148E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.1760907665344499E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.13632746602158E-2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.16755015768637E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.1609364036486601E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.1856517611097E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.14515976270223E-2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.1146623521298599E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.11513311536665E-2</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1.13499964696745E-2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1.11885616225123E-2</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1.10987490163089E-2</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1.1198521795123E-2</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1.12183279432773E-2</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1.1144074562767401E-2</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1.09583101873806E-2</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>1.09295272362545E-2</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>1.08555493820042E-2</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1.10147243465358E-2</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>1.09600679694138E-2</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>1.0979718876018099E-2</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>1.101312E-2</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>1.0909721796991401E-2</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>1.1092561204073001E-2</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>1.1066621469041801E-2</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>1.09595459325672E-2</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>1.0969465648855E-2</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>1.09269478002496E-2</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>1.11326946192821E-2</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>1.0989678663922401E-2</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>1.09051364662998E-2</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>1.0805578351241E-2</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>1.08828713509999E-2</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>1.0773723887167699E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000E-961B-4FC7-9B8A-1775915C5FCB}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>data_output_simu_model1!$BE$22:$DB$22</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.8780487804878099E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.125E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.1496062992125998E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.9138755980861202E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.9607843137254902E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.04529616724739E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.3071354705273994E-3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.5094339622641499E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.22137404580153E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8.8847322889876092E-3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5.6899004267425297E-3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>7.73218522098234E-3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>7.2854830005396696E-3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7.1135156797915997E-3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>6.7352152524122197E-3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>6.3850353287135996E-3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>6.2265934625313603E-3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>6.3121350796907097E-3</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>6.3027256157795397E-3</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>6.2381770660351497E-3</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>6.18902821503886E-3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>6.3326601081503701E-3</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>6.1866545024304703E-3</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>6.0428018778001299E-3</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>6.00991432173518E-3</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>6.2118561059531698E-3</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>6.1545320017089003E-3</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>6.0791641353861803E-3</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>5.9242502980466497E-3</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>6.0064685045433499E-3</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>6.0289730709917099E-3</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>5.8706556138018E-3</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>6.0318272568482597E-3</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>6.1863907474515901E-3</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>6.27477282736496E-3</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>6.1571331063534204E-3</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>6.1810011930018604E-3</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>6.1667195031086001E-3</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>6.0911395565650403E-3</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>6.2242169826157399E-3</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>6.1663732217033798E-3</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>6.18167594791746E-3</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>6.2501764731982597E-3</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>6.1894499385687501E-3</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>6.0818011317508702E-3</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>5.9511809626720596E-3</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>6.0058787809095003E-3</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>6.0107560898449899E-3</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>5.8987191927814204E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000F-961B-4FC7-9B8A-1775915C5FCB}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>data_output_simu_model1!$BE$23:$DB$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.9230769230769201E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.86915887850467E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.60824742268041E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.27272727272727E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.9667170953101401E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.56378600823045E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.1709601873536301E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8.4745762711864406E-3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6.2792056074766397E-3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4.8477013815948896E-3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.1275456978273704E-3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.77998920003086E-3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.82437520381845E-3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.9089568415628696E-3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.7839270508489898E-3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3.65995674596573E-3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3.7689563532395999E-3</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.9034817934966901E-3</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3.89532784996258E-3</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3.7205263384443802E-3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3.7532613809720698E-3</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3.7251146222449499E-3</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3.6516580847300701E-3</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3.7281558653330599E-3</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3.7978243771483798E-3</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>3.8252882844238101E-3</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>3.6764705882352902E-3</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>3.74237315417337E-3</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3.71808961334217E-3</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>3.5156544700113198E-3</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>3.5672515598359602E-3</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>3.6827200211685201E-3</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>3.7401611120522101E-3</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>3.7933471557432801E-3</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>3.84930248099574E-3</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>3.7331039814198202E-3</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>3.8441841861274698E-3</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>3.7395866507987101E-3</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>3.7834525846338301E-3</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>3.7151909845590499E-3</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>3.7095280441994901E-3</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>3.69757646155677E-3</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>3.7701815353305699E-3</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>3.7120557982009798E-3</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>3.6233886976405299E-3</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>3.7133171685621502E-3</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>3.72567635677412E-3</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>3.7205560722994501E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000010-961B-4FC7-9B8A-1775915C5FCB}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>data_output_simu_model1!$BE$24:$DB$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.6206896551724102E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.5862068965517199E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.8145161290322599E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.13989637305699E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.7591623036649204E-3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.3735528685361503E-3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.7351880473982498E-3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.36373633482114E-3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.6101896517544401E-3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.3895478769125002E-3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.38207787633586E-3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2.37742717802578E-3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.4176001289386699E-3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.3624745123502801E-3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2.28768769914713E-3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2.3603672276718002E-3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2.35854542409624E-3</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2.4180620277689099E-3</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.3642460454473598E-3</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2.3950898484703599E-3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2.4567049012992901E-3</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2.43394854143113E-3</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2.4581962876923402E-3</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2.4343535048522102E-3</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2.3213119637067701E-3</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2.4150444831461601E-3</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2.2669823055009399E-3</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2.2911806749376699E-3</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2.2390598245208598E-3</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2.2493881922173199E-3</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2.2656499663950098E-3</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2.3495958007955101E-3</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2.4033845157259001E-3</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>2.3718043340245701E-3</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>2.2995479606715799E-3</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>2.3275908933542799E-3</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>2.4860410798239699E-3</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>2.3606824466193199E-3</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>2.33679965770822E-3</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>2.41330585642263E-3</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>2.4206242918957798E-3</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>2.4653905376646498E-3</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>2.40051676995859E-3</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>2.3209895634220099E-3</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>2.3231465315365E-3</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>2.2950302995573299E-3</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>2.29274041910894E-3</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>2.2849990957604098E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000011-961B-4FC7-9B8A-1775915C5FCB}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="8"/>
-          <c:order val="8"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>data_output_simu_model1!$BE$25:$DB$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.1276595744680899E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.6206896551724102E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.4705882352941201E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.21543408360129E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.6457304163726203E-3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.4814340588988496E-3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.3227390927477599E-3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.5127246955737401E-3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.0723547871395599E-3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.91857941098212E-3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.6504895281707001E-3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.6416384089563501E-3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.5998177177388301E-3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.59966367872768E-3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.6385010473584901E-3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.6100409989325301E-3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.5601455615809E-3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.56304781574905E-3</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.52147858449505E-3</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.55419746210468E-3</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.53476050583096E-3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.4897728597995799E-3</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.45334074006267E-3</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.4660991228488201E-3</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1.52620188398364E-3</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1.5314682342233801E-3</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1.4963285572492601E-3</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1.53096224043743E-3</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1.4793029223754599E-3</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1.52802656434697E-3</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1.44294902707408E-3</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>1.4955977568538799E-3</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>1.5315851906723499E-3</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1.49314629579566E-3</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>1.52040016331152E-3</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>1.56716408546753E-3</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>1.55015815124828E-3</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>1.53685829590346E-3</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>1.5341514639562099E-3</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>1.5864303812696001E-3</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>1.53267574305275E-3</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>1.59193952134014E-3</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>1.5913678000310501E-3</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>1.56162464108326E-3</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>1.51968448694049E-3</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>1.5842025575165701E-3</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>1.5587214474558E-3</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>1.48452266212715E-3</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>1.5272751834668999E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000012-961B-4FC7-9B8A-1775915C5FCB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7771,13 +4927,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>657224</xdr:colOff>
+      <xdr:colOff>597460</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>136524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>546099</xdr:colOff>
+      <xdr:colOff>486335</xdr:colOff>
       <xdr:row>79</xdr:row>
       <xdr:rowOff>120649</xdr:rowOff>
     </xdr:to>
@@ -8066,8 +5222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FK45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="DN51" sqref="DN51"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O87" sqref="O87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>